<commit_message>
Reset of import limits added to varinit
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Localisation-Lo.xlsx
+++ b/suppxls/Scen_Localisation-Lo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FF2B01-0251-40EB-8158-A6CA8CF63E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD9852E-7E46-4FF6-AA27-BD634A005FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1530" yWindow="-18060" windowWidth="28770" windowHeight="15570" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
+    <workbookView xWindow="30" yWindow="630" windowWidth="28770" windowHeight="15570" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>~TFM_INS-TS</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>FX</t>
+  </si>
+  <si>
+    <t>CGE seems to break if we go to 65% imports.</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="C3:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +510,7 @@
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +520,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -549,7 +552,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
@@ -574,16 +577,19 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J5" s="7">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="K5" s="7">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="L5" s="7">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="N5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Localisation files fixed (cost update was wrong)
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Localisation-Lo.xlsx
+++ b/suppxls/Scen_Localisation-Lo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE0AFBC-38BB-4832-815A-77A0FAF85E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AE1569-2897-4891-9C6B-674EC343909C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="1560" windowWidth="24705" windowHeight="14040" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
+    <workbookView xWindow="60" yWindow="15" windowWidth="28770" windowHeight="15570" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="136">
   <si>
     <t>~TFM_INS-TS</t>
   </si>
@@ -426,6 +426,24 @@
   </si>
   <si>
     <t>cbsrv</t>
+  </si>
+  <si>
+    <t>QM</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>QINV(s-e)</t>
+  </si>
+  <si>
+    <t>Max full local</t>
+  </si>
+  <si>
+    <t>metp</t>
+  </si>
+  <si>
+    <t>Cost Increase</t>
   </si>
 </sst>
 </file>
@@ -435,7 +453,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,16 +522,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -601,15 +631,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -644,9 +690,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 13" xfId="4" xr:uid="{8D155F1E-CE31-43C4-B63E-69EA0E23AFF4}"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{114B2D43-D8F0-4A77-911E-913BD0BF594C}"/>
@@ -1027,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1C3BE-43A3-4F6E-B7BA-55F1C4F1EF02}">
-  <dimension ref="B2:BL66"/>
+  <dimension ref="B2:BL83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1097,7 @@
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="C3" s="30" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1150,27 +1199,27 @@
       </c>
       <c r="G8" s="4">
         <f>1-N32</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="H8" s="4">
         <f>G8</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="I8" s="27">
         <f t="shared" ref="I8:L8" si="2">SUMIFS(I$41:I$63,$C$41:$C$63,$E18,$F$41:$F$63,$C$3)</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="J8" s="27">
         <f t="shared" si="2"/>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="K8" s="27">
         <f t="shared" si="2"/>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="L8" s="27">
         <f t="shared" si="2"/>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
@@ -1182,27 +1231,27 @@
       </c>
       <c r="G9" s="4">
         <f>1-O32</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="H9" s="4">
         <f>G9</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="I9" s="27">
         <f t="shared" ref="I9:L9" si="3">SUMIFS(I$41:I$63,$C$41:$C$63,$E19,$F$41:$F$63,$C$3)</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="J9" s="27">
         <f t="shared" si="3"/>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="K9" s="27">
         <f t="shared" si="3"/>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="L9" s="27">
         <f t="shared" si="3"/>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
@@ -1346,27 +1395,27 @@
       </c>
       <c r="G18" s="5">
         <f>N32</f>
-        <v>0.23899999999999999</v>
+        <v>0.23934426229508196</v>
       </c>
       <c r="H18" s="5">
         <f>G18</f>
-        <v>0.23899999999999999</v>
+        <v>0.23934426229508196</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" ref="I18:L18" si="6">1-I8</f>
-        <v>0.23899999999999999</v>
+        <v>0.23934426229508199</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="6"/>
-        <v>0.23899999999999999</v>
+        <v>0.23934426229508199</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="6"/>
-        <v>0.23899999999999999</v>
+        <v>0.23934426229508199</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" si="6"/>
-        <v>0.23899999999999999</v>
+        <v>0.23934426229508199</v>
       </c>
       <c r="T18" s="12" t="s">
         <v>110</v>
@@ -1431,27 +1480,27 @@
       </c>
       <c r="G19" s="6">
         <f>O32</f>
-        <v>0.08</v>
+        <v>6.1576354679802957E-2</v>
       </c>
       <c r="H19" s="5">
         <f>G19</f>
-        <v>0.08</v>
+        <v>6.1576354679802957E-2</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" ref="I19:L19" si="7">1-I9</f>
-        <v>7.999999999999996E-2</v>
+        <v>6.1576354679802936E-2</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="7"/>
-        <v>7.999999999999996E-2</v>
+        <v>6.1576354679802936E-2</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="7"/>
-        <v>7.999999999999996E-2</v>
+        <v>6.1576354679802936E-2</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="7"/>
-        <v>7.999999999999996E-2</v>
+        <v>6.1576354679802936E-2</v>
       </c>
       <c r="T19" s="11" t="s">
         <v>111</v>
@@ -1470,27 +1519,28 @@
         <v>109</v>
       </c>
       <c r="BB22" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="BC22" s="6">
-        <f>BB22</f>
-        <v>0.1</v>
-      </c>
-      <c r="BD22" s="6">
-        <f>BC22</f>
-        <v>0.1</v>
-      </c>
-      <c r="BE22" s="6">
-        <f>BD22</f>
-        <v>0.1</v>
-      </c>
-      <c r="BF22" s="6">
-        <f>BE22</f>
-        <v>0.1</v>
-      </c>
-      <c r="BG22" s="6">
-        <f>BF22</f>
-        <v>0.1</v>
+        <f>SUMIF($F$66:$F$69,$C$3,G66:G69)</f>
+        <v>0</v>
+      </c>
+      <c r="BC22" s="4">
+        <f t="shared" ref="BC22:BG22" si="8">SUMIF($F$66:$F$69,$C$3,H66:H69)</f>
+        <v>0</v>
+      </c>
+      <c r="BD22" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BE22" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BF22" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="BG22" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="3:64" x14ac:dyDescent="0.25">
@@ -1677,7 +1727,7 @@
         <v>21</v>
       </c>
       <c r="AQ26" s="9" t="str">
-        <f t="shared" ref="AQ26:AQ49" si="8">V26</f>
+        <f t="shared" ref="AQ26:AQ49" si="9">V26</f>
         <v>ETCLEMEDU-N</v>
       </c>
       <c r="AR26" s="7">
@@ -1702,27 +1752,27 @@
         <v>ETCLEMEDU-N</v>
       </c>
       <c r="BB26">
-        <f t="shared" ref="BB26:BB65" si="9">IF($BJ26,X26*(1+$BB$22),X26)</f>
+        <f t="shared" ref="BB26:BB65" si="10">IF($BJ26,X26*(1+$BB$22),X26)</f>
         <v>51359.8538564517</v>
       </c>
       <c r="BC26" t="str">
-        <f t="shared" ref="BC26:BC49" si="10">IF(IF($BJ26,AC26*(1+BC$22),AC26)=0,"",IF($BJ26,AC26*(1+BC$22),AC26))</f>
+        <f t="shared" ref="BC26:BC49" si="11">IF(IF($BJ26,AC26*(1+BC$22),AC26)=0,"",IF($BJ26,AC26*(1+BC$22),AC26))</f>
         <v/>
       </c>
       <c r="BD26" t="str">
-        <f t="shared" ref="BD26:BD49" si="11">IF(IF($BJ26,AH26*(1+BD$22),AH26)=0,"",IF($BJ26,AH26*(1+BD$22),AH26))</f>
+        <f t="shared" ref="BD26:BD49" si="12">IF(IF($BJ26,AH26*(1+BD$22),AH26)=0,"",IF($BJ26,AH26*(1+BD$22),AH26))</f>
         <v/>
       </c>
       <c r="BE26" t="str">
-        <f t="shared" ref="BE26:BE49" si="12">IF(IF($BJ26,AM26*(1+BE$22),AM26)=0,"",IF($BJ26,AM26*(1+BE$22),AM26))</f>
+        <f t="shared" ref="BE26:BE49" si="13">IF(IF($BJ26,AM26*(1+BE$22),AM26)=0,"",IF($BJ26,AM26*(1+BE$22),AM26))</f>
         <v/>
       </c>
       <c r="BF26" t="str">
-        <f t="shared" ref="BF26:BF49" si="13">IF(IF($BJ26,AS26*(1+BF$22),AS26)=0,"",IF($BJ26,AS26*(1+BF$22),AS26))</f>
+        <f t="shared" ref="BF26:BF49" si="14">IF(IF($BJ26,AS26*(1+BF$22),AS26)=0,"",IF($BJ26,AS26*(1+BF$22),AS26))</f>
         <v/>
       </c>
       <c r="BG26" t="str">
-        <f t="shared" ref="BG26:BG49" si="14">IF(IF($BJ26,AX26*(1+BG$22),AX26)=0,"",IF($BJ26,AX26*(1+BG$22),AX26))</f>
+        <f t="shared" ref="BG26:BG49" si="15">IF(IF($BJ26,AX26*(1+BG$22),AX26)=0,"",IF($BJ26,AX26*(1+BG$22),AX26))</f>
         <v/>
       </c>
       <c r="BJ26">
@@ -1749,7 +1799,7 @@
         <v>21</v>
       </c>
       <c r="AA27" s="9" t="str">
-        <f t="shared" ref="AA27:AA49" si="15">V27</f>
+        <f t="shared" ref="AA27:AA49" si="16">V27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AB27" s="7">
@@ -1759,7 +1809,7 @@
         <v>21</v>
       </c>
       <c r="AF27" s="9" t="str">
-        <f t="shared" ref="AF27:AF49" si="16">AA27</f>
+        <f t="shared" ref="AF27:AF49" si="17">AA27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AG27" s="7">
@@ -1769,7 +1819,7 @@
         <v>21</v>
       </c>
       <c r="AK27" s="9" t="str">
-        <f t="shared" ref="AK27:AK49" si="17">AF27</f>
+        <f t="shared" ref="AK27:AK49" si="18">AF27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AL27" s="7">
@@ -1779,7 +1829,7 @@
         <v>21</v>
       </c>
       <c r="AQ27" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AR27" s="7">
@@ -1789,42 +1839,42 @@
         <v>21</v>
       </c>
       <c r="AV27" s="9" t="str">
-        <f t="shared" ref="AV27:AV49" si="18">V27</f>
+        <f t="shared" ref="AV27:AV49" si="19">V27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AW27" s="7">
         <v>2050</v>
       </c>
       <c r="AZ27" t="str">
-        <f t="shared" ref="AZ27:AZ65" si="19">U27</f>
+        <f t="shared" ref="AZ27:AZ65" si="20">U27</f>
         <v>NCAP_COST</v>
       </c>
       <c r="BA27" t="str">
-        <f t="shared" ref="BA27:BA65" si="20">V27</f>
+        <f t="shared" ref="BA27:BA65" si="21">V27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="BB27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>51359.8538564517</v>
       </c>
       <c r="BC27" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD27" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE27" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF27" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ27">
@@ -1854,7 +1904,7 @@
         <v>21</v>
       </c>
       <c r="AA28" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETCLEWATE-N</v>
       </c>
       <c r="AB28" s="7">
@@ -1864,7 +1914,7 @@
         <v>21</v>
       </c>
       <c r="AF28" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETCLEWATE-N</v>
       </c>
       <c r="AG28" s="7">
@@ -1874,7 +1924,7 @@
         <v>21</v>
       </c>
       <c r="AK28" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETCLEWATE-N</v>
       </c>
       <c r="AL28" s="7">
@@ -1884,7 +1934,7 @@
         <v>21</v>
       </c>
       <c r="AQ28" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETCLEWATE-N</v>
       </c>
       <c r="AR28" s="7">
@@ -1894,42 +1944,42 @@
         <v>21</v>
       </c>
       <c r="AV28" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETCLEWATE-N</v>
       </c>
       <c r="AW28" s="7">
         <v>2050</v>
       </c>
       <c r="AZ28" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA28" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETCLEWATE-N</v>
       </c>
       <c r="BB28">
-        <f t="shared" si="9"/>
-        <v>66921.263816000006</v>
+        <f t="shared" si="10"/>
+        <v>60837.512560000003</v>
       </c>
       <c r="BC28" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD28" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE28" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF28" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ28">
@@ -1977,7 +2027,7 @@
         <v>21</v>
       </c>
       <c r="AA29" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETCLE-CCS-N</v>
       </c>
       <c r="AB29" s="7">
@@ -1987,7 +2037,7 @@
         <v>21</v>
       </c>
       <c r="AF29" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETCLE-CCS-N</v>
       </c>
       <c r="AG29" s="7">
@@ -1997,7 +2047,7 @@
         <v>21</v>
       </c>
       <c r="AK29" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETCLE-CCS-N</v>
       </c>
       <c r="AL29" s="7">
@@ -2007,7 +2057,7 @@
         <v>21</v>
       </c>
       <c r="AQ29" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETCLE-CCS-N</v>
       </c>
       <c r="AR29" s="7">
@@ -2017,42 +2067,42 @@
         <v>21</v>
       </c>
       <c r="AV29" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETCLE-CCS-N</v>
       </c>
       <c r="AW29" s="7">
         <v>2050</v>
       </c>
       <c r="AZ29" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA29" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETCLE-CCS-N</v>
       </c>
       <c r="BB29">
-        <f t="shared" si="9"/>
-        <v>129449.205424</v>
+        <f t="shared" si="10"/>
+        <v>117681.09583999999</v>
       </c>
       <c r="BC29" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD29" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE29" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF29" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG29" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ29">
@@ -2105,7 +2155,7 @@
         <v>21</v>
       </c>
       <c r="AA30" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>EPTSTO-N</v>
       </c>
       <c r="AB30" s="7">
@@ -2115,7 +2165,7 @@
         <v>21</v>
       </c>
       <c r="AF30" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>EPTSTO-N</v>
       </c>
       <c r="AG30" s="7">
@@ -2125,7 +2175,7 @@
         <v>21</v>
       </c>
       <c r="AK30" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>EPTSTO-N</v>
       </c>
       <c r="AL30" s="7">
@@ -2135,7 +2185,7 @@
         <v>21</v>
       </c>
       <c r="AQ30" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>EPTSTO-N</v>
       </c>
       <c r="AR30" s="7">
@@ -2145,42 +2195,42 @@
         <v>21</v>
       </c>
       <c r="AV30" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>EPTSTO-N</v>
       </c>
       <c r="AW30" s="7">
         <v>2050</v>
       </c>
       <c r="AZ30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA30" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>EPTSTO-N</v>
       </c>
       <c r="BB30">
-        <f t="shared" si="9"/>
-        <v>38194.988260000006</v>
+        <f t="shared" si="10"/>
+        <v>34722.7166</v>
       </c>
       <c r="BC30" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD30" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE30" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF30" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG30" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ30">
@@ -2244,7 +2294,7 @@
         <v>21</v>
       </c>
       <c r="AA31" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETCLDFB-N</v>
       </c>
       <c r="AB31" s="7">
@@ -2254,7 +2304,7 @@
         <v>21</v>
       </c>
       <c r="AF31" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETCLDFB-N</v>
       </c>
       <c r="AG31" s="7">
@@ -2264,7 +2314,7 @@
         <v>21</v>
       </c>
       <c r="AK31" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETCLDFB-N</v>
       </c>
       <c r="AL31" s="7">
@@ -2274,7 +2324,7 @@
         <v>21</v>
       </c>
       <c r="AQ31" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETCLDFB-N</v>
       </c>
       <c r="AR31" s="7">
@@ -2284,42 +2334,42 @@
         <v>21</v>
       </c>
       <c r="AV31" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETCLDFB-N</v>
       </c>
       <c r="AW31" s="7">
         <v>2050</v>
       </c>
       <c r="AZ31" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA31" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETCLDFB-N</v>
       </c>
       <c r="BB31">
-        <f t="shared" si="9"/>
-        <v>80776.611784000008</v>
+        <f t="shared" si="10"/>
+        <v>73433.283439999999</v>
       </c>
       <c r="BC31" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD31" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE31" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF31" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG31" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ31">
@@ -2359,10 +2409,12 @@
         <v>0.52941176470588236</v>
       </c>
       <c r="N32" s="5">
-        <v>0.23899999999999999</v>
+        <f>G83</f>
+        <v>0.23934426229508196</v>
       </c>
       <c r="O32" s="24">
-        <v>0.08</v>
+        <f>G81</f>
+        <v>6.1576354679802957E-2</v>
       </c>
       <c r="T32" s="9" t="s">
         <v>37</v>
@@ -2383,7 +2435,7 @@
         <v>21</v>
       </c>
       <c r="AA32" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETNUC-N</v>
       </c>
       <c r="AB32" s="7">
@@ -2393,7 +2445,7 @@
         <v>21</v>
       </c>
       <c r="AF32" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETNUC-N</v>
       </c>
       <c r="AG32" s="7">
@@ -2403,7 +2455,7 @@
         <v>21</v>
       </c>
       <c r="AK32" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETNUC-N</v>
       </c>
       <c r="AL32" s="7">
@@ -2413,7 +2465,7 @@
         <v>21</v>
       </c>
       <c r="AQ32" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETNUC-N</v>
       </c>
       <c r="AR32" s="7">
@@ -2423,42 +2475,42 @@
         <v>21</v>
       </c>
       <c r="AV32" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETNUC-N</v>
       </c>
       <c r="AW32" s="7">
         <v>2050</v>
       </c>
       <c r="AZ32" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA32" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETNUC-N</v>
       </c>
       <c r="BB32">
-        <f t="shared" si="9"/>
-        <v>116627.07389080001</v>
+        <f t="shared" si="10"/>
+        <v>106024.612628</v>
       </c>
       <c r="BC32" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD32" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE32" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF32" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ32">
@@ -2501,7 +2553,7 @@
         <v>21</v>
       </c>
       <c r="AA33" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERSOLTC09-N</v>
       </c>
       <c r="AB33" s="7">
@@ -2514,7 +2566,7 @@
         <v>21</v>
       </c>
       <c r="AF33" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERSOLTC09-N</v>
       </c>
       <c r="AG33" s="7">
@@ -2527,7 +2579,7 @@
         <v>21</v>
       </c>
       <c r="AK33" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERSOLTC09-N</v>
       </c>
       <c r="AL33" s="7">
@@ -2540,7 +2592,7 @@
         <v>21</v>
       </c>
       <c r="AQ33" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERSOLTC09-N</v>
       </c>
       <c r="AR33" s="7">
@@ -2553,7 +2605,7 @@
         <v>21</v>
       </c>
       <c r="AV33" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERSOLTC09-N</v>
       </c>
       <c r="AW33" s="7">
@@ -2563,36 +2615,36 @@
         <v>54699.731407741099</v>
       </c>
       <c r="AZ33" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA33" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERSOLTC09-N</v>
       </c>
       <c r="BB33">
-        <f t="shared" si="9"/>
-        <v>98348.781048411969</v>
+        <f t="shared" si="10"/>
+        <v>89407.982771283598</v>
       </c>
       <c r="BC33">
-        <f t="shared" si="10"/>
-        <v>89538.224933051184</v>
+        <f t="shared" si="11"/>
+        <v>81398.386302773797</v>
       </c>
       <c r="BD33">
-        <f t="shared" si="11"/>
-        <v>74853.964740783151</v>
+        <f t="shared" si="12"/>
+        <v>68049.058855257405</v>
       </c>
       <c r="BE33">
-        <f t="shared" si="12"/>
-        <v>60169.704548515212</v>
+        <f t="shared" si="13"/>
+        <v>54699.731407741099</v>
       </c>
       <c r="BF33">
-        <f t="shared" si="13"/>
-        <v>60169.704548515212</v>
+        <f t="shared" si="14"/>
+        <v>54699.731407741099</v>
       </c>
       <c r="BG33">
-        <f t="shared" si="14"/>
-        <v>60169.704548515212</v>
+        <f t="shared" si="15"/>
+        <v>54699.731407741099</v>
       </c>
       <c r="BJ33">
         <v>1</v>
@@ -2631,7 +2683,7 @@
         <v>21</v>
       </c>
       <c r="AA34" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERSOLPCF-N</v>
       </c>
       <c r="AB34" s="7">
@@ -2644,7 +2696,7 @@
         <v>21</v>
       </c>
       <c r="AF34" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERSOLPCF-N</v>
       </c>
       <c r="AG34" s="7">
@@ -2657,7 +2709,7 @@
         <v>21</v>
       </c>
       <c r="AK34" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERSOLPCF-N</v>
       </c>
       <c r="AL34" s="7">
@@ -2670,7 +2722,7 @@
         <v>21</v>
       </c>
       <c r="AQ34" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERSOLPCF-N</v>
       </c>
       <c r="AR34" s="7">
@@ -2683,7 +2735,7 @@
         <v>21</v>
       </c>
       <c r="AV34" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERSOLPCF-N</v>
       </c>
       <c r="AW34" s="7">
@@ -2693,36 +2745,36 @@
         <v>10513.896293805299</v>
       </c>
       <c r="AZ34" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA34" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERSOLPCF-N</v>
       </c>
       <c r="BB34">
-        <f t="shared" si="9"/>
-        <v>23601.065847787562</v>
+        <f t="shared" si="10"/>
+        <v>21455.514407079601</v>
       </c>
       <c r="BC34">
-        <f t="shared" si="10"/>
-        <v>16710.377935929151</v>
+        <f t="shared" si="11"/>
+        <v>15191.2526690265</v>
       </c>
       <c r="BD34">
-        <f t="shared" si="11"/>
-        <v>15685.82797557523</v>
+        <f t="shared" si="12"/>
+        <v>14259.843614159299</v>
       </c>
       <c r="BE34">
-        <f t="shared" si="12"/>
-        <v>14736.284009203462</v>
+        <f t="shared" si="13"/>
+        <v>13396.6218265486</v>
       </c>
       <c r="BF34">
-        <f t="shared" si="13"/>
-        <v>13090.939758230072</v>
+        <f t="shared" si="14"/>
+        <v>11900.8543256637</v>
       </c>
       <c r="BG34">
-        <f t="shared" si="14"/>
-        <v>11565.285923185829</v>
+        <f t="shared" si="15"/>
+        <v>10513.896293805299</v>
       </c>
       <c r="BJ34">
         <v>1</v>
@@ -2748,7 +2800,7 @@
         <v>21</v>
       </c>
       <c r="AA35" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERSOLPCT-N</v>
       </c>
       <c r="AB35" s="7">
@@ -2761,7 +2813,7 @@
         <v>21</v>
       </c>
       <c r="AF35" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERSOLPCT-N</v>
       </c>
       <c r="AG35" s="7">
@@ -2774,7 +2826,7 @@
         <v>21</v>
       </c>
       <c r="AK35" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERSOLPCT-N</v>
       </c>
       <c r="AL35" s="7">
@@ -2787,7 +2839,7 @@
         <v>21</v>
       </c>
       <c r="AQ35" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERSOLPCT-N</v>
       </c>
       <c r="AR35" s="7">
@@ -2800,7 +2852,7 @@
         <v>21</v>
       </c>
       <c r="AV35" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERSOLPCT-N</v>
       </c>
       <c r="AW35" s="7">
@@ -2810,36 +2862,36 @@
         <v>11208.2102</v>
       </c>
       <c r="AZ35" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA35" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERSOLPCT-N</v>
       </c>
       <c r="BB35">
-        <f t="shared" si="9"/>
-        <v>25159.626800000002</v>
+        <f t="shared" si="10"/>
+        <v>22872.387999999999</v>
       </c>
       <c r="BC35">
-        <f t="shared" si="10"/>
-        <v>17813.893459999999</v>
+        <f t="shared" si="11"/>
+        <v>16194.4486</v>
       </c>
       <c r="BD35">
-        <f t="shared" si="11"/>
-        <v>16721.684540000002</v>
+        <f t="shared" si="12"/>
+        <v>15201.5314</v>
       </c>
       <c r="BE35">
-        <f t="shared" si="12"/>
-        <v>15709.434840000002</v>
+        <f t="shared" si="13"/>
+        <v>14281.304400000001</v>
       </c>
       <c r="BF35">
-        <f t="shared" si="13"/>
-        <v>13955.435780000002</v>
+        <f t="shared" si="14"/>
+        <v>12686.7598</v>
       </c>
       <c r="BG35">
-        <f t="shared" si="14"/>
-        <v>12329.031220000001</v>
+        <f t="shared" si="15"/>
+        <v>11208.2102</v>
       </c>
       <c r="BJ35">
         <v>1</v>
@@ -2865,7 +2917,7 @@
         <v>21</v>
       </c>
       <c r="AA36" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERWNDH-N</v>
       </c>
       <c r="AB36" s="7">
@@ -2878,7 +2930,7 @@
         <v>21</v>
       </c>
       <c r="AF36" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERWNDH-N</v>
       </c>
       <c r="AG36" s="7">
@@ -2891,7 +2943,7 @@
         <v>21</v>
       </c>
       <c r="AK36" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERWNDH-N</v>
       </c>
       <c r="AL36" s="7">
@@ -2904,7 +2956,7 @@
         <v>21</v>
       </c>
       <c r="AQ36" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERWNDH-N</v>
       </c>
       <c r="AR36" s="7">
@@ -2917,7 +2969,7 @@
         <v>21</v>
       </c>
       <c r="AV36" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERWNDH-N</v>
       </c>
       <c r="AW36" s="7">
@@ -2927,36 +2979,36 @@
         <v>18341.129400000002</v>
       </c>
       <c r="AZ36" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA36" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERWNDH-N</v>
       </c>
       <c r="BB36">
-        <f t="shared" si="9"/>
-        <v>26051.725920000004</v>
+        <f t="shared" si="10"/>
+        <v>23683.387200000001</v>
       </c>
       <c r="BC36">
-        <f t="shared" si="10"/>
-        <v>21265.75</v>
+        <f t="shared" si="11"/>
+        <v>19332.5</v>
       </c>
       <c r="BD36">
-        <f t="shared" si="11"/>
-        <v>21080.312660000003</v>
+        <f t="shared" si="12"/>
+        <v>19163.920600000001</v>
       </c>
       <c r="BE36">
-        <f t="shared" si="12"/>
-        <v>20896.576580000001</v>
+        <f t="shared" si="13"/>
+        <v>18996.8878</v>
       </c>
       <c r="BF36">
-        <f t="shared" si="13"/>
-        <v>20532.506940000003</v>
+        <f t="shared" si="14"/>
+        <v>18665.915400000002</v>
       </c>
       <c r="BG36">
-        <f t="shared" si="14"/>
-        <v>20175.242340000004</v>
+        <f t="shared" si="15"/>
+        <v>18341.129400000002</v>
       </c>
       <c r="BJ36">
         <v>1</v>
@@ -2982,7 +3034,7 @@
         <v>21</v>
       </c>
       <c r="AA37" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETGICGT-N</v>
       </c>
       <c r="AB37" s="7">
@@ -2992,7 +3044,7 @@
         <v>21</v>
       </c>
       <c r="AF37" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETGICGT-N</v>
       </c>
       <c r="AG37" s="7">
@@ -3002,7 +3054,7 @@
         <v>21</v>
       </c>
       <c r="AK37" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETGICGT-N</v>
       </c>
       <c r="AL37" s="7">
@@ -3012,7 +3064,7 @@
         <v>21</v>
       </c>
       <c r="AQ37" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETGICGT-N</v>
       </c>
       <c r="AR37" s="7">
@@ -3022,42 +3074,42 @@
         <v>21</v>
       </c>
       <c r="AV37" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETGICGT-N</v>
       </c>
       <c r="AW37" s="7">
         <v>2050</v>
       </c>
       <c r="AZ37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA37" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETGICGT-N</v>
       </c>
       <c r="BB37">
-        <f t="shared" si="9"/>
-        <v>15423.436336000001</v>
+        <f t="shared" si="10"/>
+        <v>14021.305759999999</v>
       </c>
       <c r="BC37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD37" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE37" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ37">
@@ -3087,7 +3139,7 @@
         <v>21</v>
       </c>
       <c r="AA38" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETHGNGT-N</v>
       </c>
       <c r="AB38" s="7">
@@ -3097,7 +3149,7 @@
         <v>21</v>
       </c>
       <c r="AF38" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETHGNGT-N</v>
       </c>
       <c r="AG38" s="7">
@@ -3107,7 +3159,7 @@
         <v>21</v>
       </c>
       <c r="AK38" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETHGNGT-N</v>
       </c>
       <c r="AL38" s="7">
@@ -3117,7 +3169,7 @@
         <v>21</v>
       </c>
       <c r="AQ38" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETHGNGT-N</v>
       </c>
       <c r="AR38" s="7">
@@ -3127,42 +3179,42 @@
         <v>21</v>
       </c>
       <c r="AV38" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETHGNGT-N</v>
       </c>
       <c r="AW38" s="7">
         <v>2050</v>
       </c>
       <c r="AZ38" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA38" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETHGNGT-N</v>
       </c>
       <c r="BB38">
-        <f t="shared" si="9"/>
-        <v>42057.954400000002</v>
+        <f t="shared" si="10"/>
+        <v>38234.504000000001</v>
       </c>
       <c r="BC38" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF38" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG38" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ38">
@@ -3189,7 +3241,7 @@
         <v>21</v>
       </c>
       <c r="AA39" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETGICCC-N</v>
       </c>
       <c r="AB39" s="7">
@@ -3199,7 +3251,7 @@
         <v>21</v>
       </c>
       <c r="AF39" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETGICCC-N</v>
       </c>
       <c r="AG39" s="7">
@@ -3209,7 +3261,7 @@
         <v>21</v>
       </c>
       <c r="AK39" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETGICCC-N</v>
       </c>
       <c r="AL39" s="7">
@@ -3219,7 +3271,7 @@
         <v>21</v>
       </c>
       <c r="AQ39" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETGICCC-N</v>
       </c>
       <c r="AR39" s="7">
@@ -3229,42 +3281,42 @@
         <v>21</v>
       </c>
       <c r="AV39" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETGICCC-N</v>
       </c>
       <c r="AW39" s="7">
         <v>2050</v>
       </c>
       <c r="AZ39" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA39" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETGICCC-N</v>
       </c>
       <c r="BB39">
-        <f t="shared" si="9"/>
-        <v>16936.357416000003</v>
+        <f t="shared" si="10"/>
+        <v>15396.688560000001</v>
       </c>
       <c r="BC39" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD39" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE39" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF39" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG39" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ39">
@@ -3275,6 +3327,24 @@
       <c r="C40" s="10" t="s">
         <v>116</v>
       </c>
+      <c r="G40" s="2">
+        <v>2017</v>
+      </c>
+      <c r="H40" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I40">
+        <v>2025</v>
+      </c>
+      <c r="J40" s="2">
+        <v>2030</v>
+      </c>
+      <c r="K40" s="2">
+        <v>2040</v>
+      </c>
+      <c r="L40" s="2">
+        <v>2050</v>
+      </c>
       <c r="T40" s="9" t="s">
         <v>53</v>
       </c>
@@ -3294,7 +3364,7 @@
         <v>21</v>
       </c>
       <c r="AA40" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETGICCC-CCS-N</v>
       </c>
       <c r="AB40" s="7">
@@ -3304,7 +3374,7 @@
         <v>21</v>
       </c>
       <c r="AF40" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETGICCC-CCS-N</v>
       </c>
       <c r="AG40" s="7">
@@ -3314,7 +3384,7 @@
         <v>21</v>
       </c>
       <c r="AK40" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETGICCC-CCS-N</v>
       </c>
       <c r="AL40" s="7">
@@ -3324,7 +3394,7 @@
         <v>21</v>
       </c>
       <c r="AQ40" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETGICCC-CCS-N</v>
       </c>
       <c r="AR40" s="7">
@@ -3334,42 +3404,42 @@
         <v>21</v>
       </c>
       <c r="AV40" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETGICCC-CCS-N</v>
       </c>
       <c r="AW40" s="7">
         <v>2050</v>
       </c>
       <c r="AZ40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETGICCC-CCS-N</v>
       </c>
       <c r="BB40">
-        <f t="shared" si="9"/>
-        <v>37216.186832000007</v>
+        <f t="shared" si="10"/>
+        <v>33832.897120000001</v>
       </c>
       <c r="BC40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ40">
@@ -3422,7 +3492,7 @@
         <v>21</v>
       </c>
       <c r="AA41" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ETGICEN-N</v>
       </c>
       <c r="AB41" s="7">
@@ -3432,7 +3502,7 @@
         <v>21</v>
       </c>
       <c r="AF41" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ETGICEN-N</v>
       </c>
       <c r="AG41" s="7">
@@ -3442,7 +3512,7 @@
         <v>21</v>
       </c>
       <c r="AK41" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ETGICEN-N</v>
       </c>
       <c r="AL41" s="7">
@@ -3452,7 +3522,7 @@
         <v>21</v>
       </c>
       <c r="AQ41" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ETGICEN-N</v>
       </c>
       <c r="AR41" s="7">
@@ -3462,42 +3532,42 @@
         <v>21</v>
       </c>
       <c r="AV41" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ETGICEN-N</v>
       </c>
       <c r="AW41" s="7">
         <v>2050</v>
       </c>
       <c r="AZ41" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA41" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETGICEN-N</v>
       </c>
       <c r="BB41">
-        <f t="shared" si="9"/>
-        <v>24062.967984000003</v>
+        <f t="shared" si="10"/>
+        <v>21875.425439999999</v>
       </c>
       <c r="BC41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD41" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE41" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG41" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ41">
@@ -3551,7 +3621,7 @@
         <v>21</v>
       </c>
       <c r="AA42" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERBIO-N</v>
       </c>
       <c r="AB42" s="7">
@@ -3561,7 +3631,7 @@
         <v>21</v>
       </c>
       <c r="AF42" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERBIO-N</v>
       </c>
       <c r="AG42" s="7">
@@ -3571,7 +3641,7 @@
         <v>21</v>
       </c>
       <c r="AK42" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERBIO-N</v>
       </c>
       <c r="AL42" s="7">
@@ -3581,7 +3651,7 @@
         <v>21</v>
       </c>
       <c r="AQ42" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERBIO-N</v>
       </c>
       <c r="AR42" s="7">
@@ -3591,42 +3661,42 @@
         <v>21</v>
       </c>
       <c r="AV42" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERBIO-N</v>
       </c>
       <c r="AW42" s="7">
         <v>2050</v>
       </c>
       <c r="AZ42" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA42" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERBIO-N</v>
       </c>
       <c r="BB42">
-        <f t="shared" si="9"/>
-        <v>32173.281782644972</v>
+        <f t="shared" si="10"/>
+        <v>29248.437984222699</v>
       </c>
       <c r="BC42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD42" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF42" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG42" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ42">
@@ -3680,7 +3750,7 @@
         <v>21</v>
       </c>
       <c r="AA43" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERBIG-N</v>
       </c>
       <c r="AB43" s="7">
@@ -3690,7 +3760,7 @@
         <v>21</v>
       </c>
       <c r="AF43" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERBIG-N</v>
       </c>
       <c r="AG43" s="7">
@@ -3700,7 +3770,7 @@
         <v>21</v>
       </c>
       <c r="AK43" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERBIG-N</v>
       </c>
       <c r="AL43" s="7">
@@ -3710,7 +3780,7 @@
         <v>21</v>
       </c>
       <c r="AQ43" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERBIG-N</v>
       </c>
       <c r="AR43" s="7">
@@ -3720,42 +3790,42 @@
         <v>21</v>
       </c>
       <c r="AV43" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERBIG-N</v>
       </c>
       <c r="AW43" s="7">
         <v>2050</v>
       </c>
       <c r="AZ43" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA43" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERBIG-N</v>
       </c>
       <c r="BB43">
-        <f t="shared" si="9"/>
-        <v>32173.281782644972</v>
+        <f t="shared" si="10"/>
+        <v>29248.437984222699</v>
       </c>
       <c r="BC43" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD43" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="BE43" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BF43" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="BG43" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="BJ43">
@@ -3779,19 +3849,19 @@
         <v>0.47058823529411764</v>
       </c>
       <c r="I44" s="5">
-        <f t="shared" ref="I44:L44" si="21">H44</f>
+        <f t="shared" ref="I44:L44" si="22">H44</f>
         <v>0.47058823529411764</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.47058823529411764</v>
       </c>
       <c r="K44" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.47058823529411764</v>
       </c>
       <c r="L44" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.47058823529411764</v>
       </c>
       <c r="N44" t="s">
@@ -3816,7 +3886,7 @@
         <v>21</v>
       </c>
       <c r="AA44" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ESTSUTL</v>
       </c>
       <c r="AB44" s="7">
@@ -3829,7 +3899,7 @@
         <v>21</v>
       </c>
       <c r="AF44" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ESTSUTL</v>
       </c>
       <c r="AG44" s="7">
@@ -3842,7 +3912,7 @@
         <v>21</v>
       </c>
       <c r="AK44" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ESTSUTL</v>
       </c>
       <c r="AL44" s="7">
@@ -3855,7 +3925,7 @@
         <v>21</v>
       </c>
       <c r="AQ44" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ESTSUTL</v>
       </c>
       <c r="AR44" s="7">
@@ -3868,7 +3938,7 @@
         <v>21</v>
       </c>
       <c r="AV44" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ESTSUTL</v>
       </c>
       <c r="AW44" s="7">
@@ -3878,36 +3948,36 @@
         <v>15417.019777003599</v>
       </c>
       <c r="AZ44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA44" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ESTSUTL</v>
       </c>
       <c r="BB44">
-        <f t="shared" si="9"/>
-        <v>46216.813456000003</v>
+        <f t="shared" si="10"/>
+        <v>42015.284959999997</v>
       </c>
       <c r="BC44">
-        <f t="shared" si="10"/>
-        <v>29626.392114015511</v>
+        <f t="shared" si="11"/>
+        <v>26933.083740014099</v>
       </c>
       <c r="BD44">
-        <f t="shared" si="11"/>
-        <v>29250.992238274401</v>
+        <f t="shared" si="12"/>
+        <v>26591.811125704</v>
       </c>
       <c r="BE44">
-        <f t="shared" si="12"/>
-        <v>24519.026135938511</v>
+        <f t="shared" si="13"/>
+        <v>22290.023759944099</v>
       </c>
       <c r="BF44">
-        <f t="shared" si="13"/>
-        <v>20738.00984562857</v>
+        <f t="shared" si="14"/>
+        <v>18852.7362232987</v>
       </c>
       <c r="BG44">
-        <f t="shared" si="14"/>
-        <v>16958.721754703962</v>
+        <f t="shared" si="15"/>
+        <v>15417.019777003599</v>
       </c>
       <c r="BJ44">
         <v>1</v>
@@ -3933,7 +4003,7 @@
         <v>21</v>
       </c>
       <c r="AA45" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERSOLPRA-N</v>
       </c>
       <c r="AB45" s="7">
@@ -3946,7 +4016,7 @@
         <v>21</v>
       </c>
       <c r="AF45" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERSOLPRA-N</v>
       </c>
       <c r="AG45" s="7">
@@ -3959,7 +4029,7 @@
         <v>21</v>
       </c>
       <c r="AK45" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERSOLPRA-N</v>
       </c>
       <c r="AL45" s="7">
@@ -3972,7 +4042,7 @@
         <v>21</v>
       </c>
       <c r="AQ45" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERSOLPRA-N</v>
       </c>
       <c r="AR45" s="7">
@@ -3985,7 +4055,7 @@
         <v>21</v>
       </c>
       <c r="AV45" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERSOLPRA-N</v>
       </c>
       <c r="AW45" s="7">
@@ -3995,36 +4065,36 @@
         <v>12196.119700814201</v>
       </c>
       <c r="AZ45" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA45" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERSOLPRA-N</v>
       </c>
       <c r="BB45">
-        <f t="shared" si="9"/>
-        <v>27377.236383433643</v>
+        <f t="shared" si="10"/>
+        <v>24888.396712212401</v>
       </c>
       <c r="BC45">
-        <f t="shared" si="10"/>
-        <v>19384.038405677991</v>
+        <f t="shared" si="11"/>
+        <v>17621.853096070899</v>
       </c>
       <c r="BD45">
-        <f t="shared" si="11"/>
-        <v>18195.560451667283</v>
+        <f t="shared" si="12"/>
+        <v>16541.418592424801</v>
       </c>
       <c r="BE45">
-        <f t="shared" si="12"/>
-        <v>17094.089450676041</v>
+        <f t="shared" si="13"/>
+        <v>15540.0813187964</v>
       </c>
       <c r="BF45">
-        <f t="shared" si="13"/>
-        <v>15185.490119546892</v>
+        <f t="shared" si="14"/>
+        <v>13804.9910177699</v>
       </c>
       <c r="BG45">
-        <f t="shared" si="14"/>
-        <v>13415.731670895622</v>
+        <f t="shared" si="15"/>
+        <v>12196.119700814201</v>
       </c>
       <c r="BJ45">
         <v>1</v>
@@ -4050,7 +4120,7 @@
         <v>21</v>
       </c>
       <c r="AA46" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERSOLPRM-N</v>
       </c>
       <c r="AB46" s="7">
@@ -4063,7 +4133,7 @@
         <v>21</v>
       </c>
       <c r="AF46" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERSOLPRM-N</v>
       </c>
       <c r="AG46" s="7">
@@ -4076,7 +4146,7 @@
         <v>21</v>
       </c>
       <c r="AK46" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERSOLPRM-N</v>
       </c>
       <c r="AL46" s="7">
@@ -4089,7 +4159,7 @@
         <v>21</v>
       </c>
       <c r="AQ46" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERSOLPRM-N</v>
       </c>
       <c r="AR46" s="7">
@@ -4102,7 +4172,7 @@
         <v>21</v>
       </c>
       <c r="AV46" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERSOLPRM-N</v>
       </c>
       <c r="AW46" s="7">
@@ -4112,36 +4182,36 @@
         <v>12196.119700814201</v>
       </c>
       <c r="AZ46" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA46" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERSOLPRM-N</v>
       </c>
       <c r="BB46">
-        <f t="shared" si="9"/>
-        <v>27377.236383433643</v>
+        <f t="shared" si="10"/>
+        <v>24888.396712212401</v>
       </c>
       <c r="BC46">
-        <f t="shared" si="10"/>
-        <v>19384.038405677991</v>
+        <f t="shared" si="11"/>
+        <v>17621.853096070899</v>
       </c>
       <c r="BD46">
-        <f t="shared" si="11"/>
-        <v>18195.560451667283</v>
+        <f t="shared" si="12"/>
+        <v>16541.418592424801</v>
       </c>
       <c r="BE46">
-        <f t="shared" si="12"/>
-        <v>17094.089450676041</v>
+        <f t="shared" si="13"/>
+        <v>15540.0813187964</v>
       </c>
       <c r="BF46">
-        <f t="shared" si="13"/>
-        <v>15185.490119546892</v>
+        <f t="shared" si="14"/>
+        <v>13804.9910177699</v>
       </c>
       <c r="BG46">
-        <f t="shared" si="14"/>
-        <v>13415.731670895622</v>
+        <f t="shared" si="15"/>
+        <v>12196.119700814201</v>
       </c>
       <c r="BJ46">
         <v>1</v>
@@ -4170,7 +4240,7 @@
         <v>21</v>
       </c>
       <c r="AA47" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERSOLPRC-N</v>
       </c>
       <c r="AB47" s="7">
@@ -4183,7 +4253,7 @@
         <v>21</v>
       </c>
       <c r="AF47" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERSOLPRC-N</v>
       </c>
       <c r="AG47" s="7">
@@ -4196,7 +4266,7 @@
         <v>21</v>
       </c>
       <c r="AK47" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERSOLPRC-N</v>
       </c>
       <c r="AL47" s="7">
@@ -4209,7 +4279,7 @@
         <v>21</v>
       </c>
       <c r="AQ47" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERSOLPRC-N</v>
       </c>
       <c r="AR47" s="7">
@@ -4222,7 +4292,7 @@
         <v>21</v>
       </c>
       <c r="AV47" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERSOLPRC-N</v>
       </c>
       <c r="AW47" s="7">
@@ -4232,36 +4302,36 @@
         <v>12196.119700814201</v>
       </c>
       <c r="AZ47" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA47" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERSOLPRC-N</v>
       </c>
       <c r="BB47">
-        <f t="shared" si="9"/>
-        <v>27377.236383433643</v>
+        <f t="shared" si="10"/>
+        <v>24888.396712212401</v>
       </c>
       <c r="BC47">
-        <f t="shared" si="10"/>
-        <v>19384.038405677991</v>
+        <f t="shared" si="11"/>
+        <v>17621.853096070899</v>
       </c>
       <c r="BD47">
-        <f t="shared" si="11"/>
-        <v>18195.560451667283</v>
+        <f t="shared" si="12"/>
+        <v>16541.418592424801</v>
       </c>
       <c r="BE47">
-        <f t="shared" si="12"/>
-        <v>17094.089450676041</v>
+        <f t="shared" si="13"/>
+        <v>15540.0813187964</v>
       </c>
       <c r="BF47">
-        <f t="shared" si="13"/>
-        <v>15185.490119546892</v>
+        <f t="shared" si="14"/>
+        <v>13804.9910177699</v>
       </c>
       <c r="BG47">
-        <f t="shared" si="14"/>
-        <v>13415.731670895622</v>
+        <f t="shared" si="15"/>
+        <v>12196.119700814201</v>
       </c>
       <c r="BJ47">
         <v>1</v>
@@ -4313,7 +4383,7 @@
         <v>21</v>
       </c>
       <c r="AA48" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERSOLPRR-N</v>
       </c>
       <c r="AB48" s="7">
@@ -4326,7 +4396,7 @@
         <v>21</v>
       </c>
       <c r="AF48" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERSOLPRR-N</v>
       </c>
       <c r="AG48" s="7">
@@ -4339,7 +4409,7 @@
         <v>21</v>
       </c>
       <c r="AK48" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERSOLPRR-N</v>
       </c>
       <c r="AL48" s="7">
@@ -4352,7 +4422,7 @@
         <v>21</v>
       </c>
       <c r="AQ48" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERSOLPRR-N</v>
       </c>
       <c r="AR48" s="7">
@@ -4365,7 +4435,7 @@
         <v>21</v>
       </c>
       <c r="AV48" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERSOLPRR-N</v>
       </c>
       <c r="AW48" s="7">
@@ -4375,36 +4445,36 @@
         <v>18399.318514159299</v>
       </c>
       <c r="AZ48" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA48" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERSOLPRR-N</v>
       </c>
       <c r="BB48">
-        <f t="shared" si="9"/>
-        <v>41301.865233628349</v>
+        <f t="shared" si="10"/>
+        <v>37547.150212389402</v>
       </c>
       <c r="BC48">
-        <f t="shared" si="10"/>
-        <v>29243.16138787604</v>
+        <f t="shared" si="11"/>
+        <v>26584.692170796399</v>
       </c>
       <c r="BD48">
-        <f t="shared" si="11"/>
-        <v>27450.198957256682</v>
+        <f t="shared" si="12"/>
+        <v>24954.7263247788</v>
       </c>
       <c r="BE48">
-        <f t="shared" si="12"/>
-        <v>25788.49701610611</v>
+        <f t="shared" si="13"/>
+        <v>23444.088196460099</v>
       </c>
       <c r="BF48">
-        <f t="shared" si="13"/>
-        <v>22909.14457690265</v>
+        <f t="shared" si="14"/>
+        <v>20826.4950699115</v>
       </c>
       <c r="BG48">
-        <f t="shared" si="14"/>
-        <v>20239.25036557523</v>
+        <f t="shared" si="15"/>
+        <v>18399.318514159299</v>
       </c>
       <c r="BJ48">
         <v>1</v>
@@ -4457,7 +4527,7 @@
         <v>21</v>
       </c>
       <c r="AA49" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>ERSOLPRI-N</v>
       </c>
       <c r="AB49" s="7">
@@ -4470,7 +4540,7 @@
         <v>21</v>
       </c>
       <c r="AF49" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>ERSOLPRI-N</v>
       </c>
       <c r="AG49" s="7">
@@ -4483,7 +4553,7 @@
         <v>21</v>
       </c>
       <c r="AK49" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>ERSOLPRI-N</v>
       </c>
       <c r="AL49" s="7">
@@ -4496,7 +4566,7 @@
         <v>21</v>
       </c>
       <c r="AQ49" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>ERSOLPRI-N</v>
       </c>
       <c r="AR49" s="7">
@@ -4509,7 +4579,7 @@
         <v>21</v>
       </c>
       <c r="AV49" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>ERSOLPRI-N</v>
       </c>
       <c r="AW49" s="7">
@@ -4519,36 +4589,36 @@
         <v>12196.119700814201</v>
       </c>
       <c r="AZ49" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA49" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ERSOLPRI-N</v>
       </c>
       <c r="BB49">
-        <f t="shared" si="9"/>
-        <v>27377.236383433643</v>
+        <f t="shared" si="10"/>
+        <v>24888.396712212401</v>
       </c>
       <c r="BC49">
-        <f t="shared" si="10"/>
-        <v>19384.038405677991</v>
+        <f t="shared" si="11"/>
+        <v>17621.853096070899</v>
       </c>
       <c r="BD49">
-        <f t="shared" si="11"/>
-        <v>18195.560451667283</v>
+        <f t="shared" si="12"/>
+        <v>16541.418592424801</v>
       </c>
       <c r="BE49">
-        <f t="shared" si="12"/>
-        <v>17094.089450676041</v>
+        <f t="shared" si="13"/>
+        <v>15540.0813187964</v>
       </c>
       <c r="BF49">
-        <f t="shared" si="13"/>
-        <v>15185.490119546892</v>
+        <f t="shared" si="14"/>
+        <v>13804.9910177699</v>
       </c>
       <c r="BG49">
-        <f t="shared" si="14"/>
-        <v>13415.731670895622</v>
+        <f t="shared" si="15"/>
+        <v>12196.119700814201</v>
       </c>
       <c r="BJ49">
         <v>1</v>
@@ -4610,16 +4680,16 @@
       <c r="AV50" s="9"/>
       <c r="AW50" s="7"/>
       <c r="AZ50" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA50" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETRANS</v>
       </c>
       <c r="BB50">
-        <f t="shared" si="9"/>
-        <v>7658.4609194379227</v>
+        <f t="shared" si="10"/>
+        <v>6962.23719948902</v>
       </c>
       <c r="BJ50">
         <v>1</v>
@@ -4642,19 +4712,19 @@
         <v>0.47538200339558578</v>
       </c>
       <c r="I51" s="5">
-        <f t="shared" ref="I51:L51" si="22">H51</f>
+        <f t="shared" ref="I51:L51" si="23">H51</f>
         <v>0.47538200339558578</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.47538200339558578</v>
       </c>
       <c r="K51" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.47538200339558578</v>
       </c>
       <c r="L51" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.47538200339558578</v>
       </c>
       <c r="N51" t="s">
@@ -4682,16 +4752,16 @@
       <c r="AV51" s="9"/>
       <c r="AW51" s="7"/>
       <c r="AZ51" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA51" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>ETRANSDUM</v>
       </c>
       <c r="BB51">
-        <f t="shared" si="9"/>
-        <v>3402.52</v>
+        <f t="shared" si="10"/>
+        <v>3093.2</v>
       </c>
       <c r="BJ51">
         <v>1</v>
@@ -4720,16 +4790,16 @@
       <c r="AV52" s="9"/>
       <c r="AW52" s="7"/>
       <c r="AZ52" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA52" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XAGRELC</v>
       </c>
       <c r="BB52">
-        <f t="shared" si="9"/>
-        <v>44757.091212415566</v>
+        <f t="shared" si="10"/>
+        <v>40688.264738559599</v>
       </c>
       <c r="BJ52">
         <v>1</v>
@@ -4761,16 +4831,16 @@
       <c r="AV53" s="9"/>
       <c r="AW53" s="7"/>
       <c r="AZ53" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA53" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XCOMELC</v>
       </c>
       <c r="BB53">
-        <f t="shared" si="9"/>
-        <v>22378.545678702401</v>
+        <f t="shared" si="10"/>
+        <v>20344.132435184001</v>
       </c>
       <c r="BJ53">
         <v>1</v>
@@ -4785,24 +4855,31 @@
       </c>
       <c r="G54" s="6">
         <f>1-O32</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="H54" s="6">
-        <f t="shared" ref="H54:I56" si="23">G54</f>
-        <v>0.92</v>
+        <f t="shared" ref="H54:I56" si="24">G54</f>
+        <v>0.93842364532019706</v>
       </c>
       <c r="I54" s="15">
-        <f t="shared" si="23"/>
-        <v>0.92</v>
+        <f t="shared" si="24"/>
+        <v>0.93842364532019706</v>
       </c>
       <c r="J54" s="15">
-        <v>0.95</v>
+        <f>I54+$O$54</f>
+        <v>0.94827586206896552</v>
       </c>
       <c r="K54" s="15">
-        <v>0.98</v>
+        <f t="shared" ref="K54:K55" si="25">J54</f>
+        <v>0.94827586206896552</v>
       </c>
       <c r="L54" s="15">
-        <v>0.98</v>
+        <f t="shared" ref="L54:L55" si="26">K54</f>
+        <v>0.94827586206896552</v>
+      </c>
+      <c r="O54" s="5">
+        <f>J81</f>
+        <v>9.852216748768473E-3</v>
       </c>
       <c r="T54" s="9" t="s">
         <v>81</v>
@@ -4826,16 +4903,16 @@
       <c r="AV54" s="9"/>
       <c r="AW54" s="7"/>
       <c r="AZ54" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA54" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XICPELC</v>
       </c>
       <c r="BB54">
-        <f t="shared" si="9"/>
-        <v>10637.519114867559</v>
+        <f t="shared" si="10"/>
+        <v>9670.4719226068701</v>
       </c>
       <c r="BJ54">
         <v>1</v>
@@ -4850,26 +4927,27 @@
       </c>
       <c r="G55" s="6">
         <f>G54</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="H55" s="6">
-        <f t="shared" si="23"/>
-        <v>0.92</v>
+        <f t="shared" si="24"/>
+        <v>0.93842364532019706</v>
       </c>
       <c r="I55" s="15">
-        <f t="shared" si="23"/>
-        <v>0.92</v>
+        <f t="shared" si="24"/>
+        <v>0.93842364532019706</v>
       </c>
       <c r="J55" s="15">
-        <f>J54</f>
-        <v>0.95</v>
+        <f>I55+$O$54</f>
+        <v>0.94827586206896552</v>
       </c>
       <c r="K55" s="15">
-        <f>J55</f>
-        <v>0.95</v>
+        <f t="shared" si="25"/>
+        <v>0.94827586206896552</v>
       </c>
       <c r="L55" s="15">
-        <v>0.98</v>
+        <f t="shared" si="26"/>
+        <v>0.94827586206896552</v>
       </c>
       <c r="T55" s="9" t="s">
         <v>83</v>
@@ -4893,16 +4971,16 @@
       <c r="AV55" s="9"/>
       <c r="AW55" s="7"/>
       <c r="AZ55" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA55" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XIFAELC</v>
       </c>
       <c r="BB55">
-        <f t="shared" si="9"/>
-        <v>10637.519114867559</v>
+        <f t="shared" si="10"/>
+        <v>9670.4719226068701</v>
       </c>
       <c r="BJ55">
         <v>1</v>
@@ -4917,23 +4995,23 @@
       </c>
       <c r="G56" s="6">
         <f>G55</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="H56" s="6">
-        <f t="shared" si="23"/>
-        <v>0.92</v>
+        <f t="shared" si="24"/>
+        <v>0.93842364532019706</v>
       </c>
       <c r="I56" s="15">
-        <f t="shared" si="23"/>
-        <v>0.92</v>
+        <f t="shared" si="24"/>
+        <v>0.93842364532019706</v>
       </c>
       <c r="J56" s="15">
         <f>J55</f>
-        <v>0.95</v>
+        <v>0.94827586206896552</v>
       </c>
       <c r="K56" s="15">
         <f>K55</f>
-        <v>0.95</v>
+        <v>0.94827586206896552</v>
       </c>
       <c r="L56" s="15">
         <v>0.95</v>
@@ -4960,16 +5038,16 @@
       <c r="AV56" s="9"/>
       <c r="AW56" s="7"/>
       <c r="AZ56" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA56" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XIFBELC</v>
       </c>
       <c r="BB56">
-        <f t="shared" si="9"/>
-        <v>17090.552455521491</v>
+        <f t="shared" si="10"/>
+        <v>15536.865868655899</v>
       </c>
       <c r="BJ56">
         <v>1</v>
@@ -4984,27 +5062,27 @@
       </c>
       <c r="G57" s="6">
         <f>G56</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="H57" s="6">
         <f>H56</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="I57" s="6">
         <f>H57</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="J57" s="6">
         <f>I57</f>
-        <v>0.92</v>
+        <v>0.93842364532019706</v>
       </c>
       <c r="K57" s="6">
-        <f t="shared" ref="K57:L57" si="24">J57</f>
-        <v>0.92</v>
+        <f t="shared" ref="K57:L57" si="27">J57</f>
+        <v>0.93842364532019706</v>
       </c>
       <c r="L57" s="6">
-        <f t="shared" si="24"/>
-        <v>0.92</v>
+        <f t="shared" si="27"/>
+        <v>0.93842364532019706</v>
       </c>
       <c r="N57" t="s">
         <v>128</v>
@@ -5025,16 +5103,16 @@
         <v>9670.4719226068701</v>
       </c>
       <c r="AZ57" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA57" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XIISELC</v>
       </c>
       <c r="BB57">
-        <f t="shared" si="9"/>
-        <v>10637.519114867559</v>
+        <f t="shared" si="10"/>
+        <v>9670.4719226068701</v>
       </c>
       <c r="BJ57">
         <v>1</v>
@@ -5057,16 +5135,16 @@
         <v>9670.4719226068701</v>
       </c>
       <c r="AZ58" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA58" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XIMIELC</v>
       </c>
       <c r="BB58">
-        <f t="shared" si="9"/>
-        <v>10637.519114867559</v>
+        <f t="shared" si="10"/>
+        <v>9670.4719226068701</v>
       </c>
       <c r="BJ58">
         <v>1</v>
@@ -5092,16 +5170,16 @@
         <v>9670.4719226068701</v>
       </c>
       <c r="AZ59" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA59" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XINFELC</v>
       </c>
       <c r="BB59">
-        <f t="shared" si="9"/>
-        <v>10637.519114867559</v>
+        <f t="shared" si="10"/>
+        <v>9670.4719226068701</v>
       </c>
       <c r="BJ59">
         <v>1</v>
@@ -5116,30 +5194,31 @@
       </c>
       <c r="G60" s="6">
         <f>1-N32</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="H60" s="6">
-        <f t="shared" ref="H60:I62" si="25">G60</f>
-        <v>0.76100000000000001</v>
+        <f t="shared" ref="H60:I62" si="28">G60</f>
+        <v>0.76065573770491801</v>
       </c>
       <c r="I60" s="15">
-        <f t="shared" si="25"/>
-        <v>0.76100000000000001</v>
+        <f t="shared" si="28"/>
+        <v>0.76065573770491801</v>
       </c>
       <c r="J60" s="15">
         <f>I60+$O$60</f>
-        <v>0.78700000000000003</v>
+        <v>0.78098360655737697</v>
       </c>
       <c r="K60" s="15">
-        <f t="shared" ref="K60:L63" si="26">J60</f>
-        <v>0.78700000000000003</v>
+        <f t="shared" ref="K60:L63" si="29">J60</f>
+        <v>0.78098360655737697</v>
       </c>
       <c r="L60" s="15">
-        <f t="shared" si="26"/>
-        <v>0.78700000000000003</v>
+        <f t="shared" si="29"/>
+        <v>0.78098360655737697</v>
       </c>
       <c r="O60" s="28">
-        <v>2.5999999999999999E-2</v>
+        <f>J83</f>
+        <v>2.0327868852459016E-2</v>
       </c>
       <c r="T60" s="9" t="s">
         <v>93</v>
@@ -5157,16 +5236,16 @@
         <v>9670.4719226068701</v>
       </c>
       <c r="AZ60" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA60" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XINMELC</v>
       </c>
       <c r="BB60">
-        <f t="shared" si="9"/>
-        <v>10637.519114867559</v>
+        <f t="shared" si="10"/>
+        <v>9670.4719226068701</v>
       </c>
       <c r="BJ60">
         <v>1</v>
@@ -5182,27 +5261,27 @@
       </c>
       <c r="G61" s="6">
         <f>G60</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="H61" s="6">
-        <f t="shared" si="25"/>
-        <v>0.76100000000000001</v>
+        <f t="shared" si="28"/>
+        <v>0.76065573770491801</v>
       </c>
       <c r="I61" s="15">
-        <f t="shared" si="25"/>
-        <v>0.76100000000000001</v>
+        <f t="shared" si="28"/>
+        <v>0.76065573770491801</v>
       </c>
       <c r="J61" s="15">
         <f>J60</f>
-        <v>0.78700000000000003</v>
+        <v>0.78098360655737697</v>
       </c>
       <c r="K61" s="15">
-        <f t="shared" si="26"/>
-        <v>0.78700000000000003</v>
+        <f t="shared" si="29"/>
+        <v>0.78098360655737697</v>
       </c>
       <c r="L61" s="15">
-        <f t="shared" si="26"/>
-        <v>0.78700000000000003</v>
+        <f t="shared" si="29"/>
+        <v>0.78098360655737697</v>
       </c>
       <c r="T61" s="9" t="s">
         <v>95</v>
@@ -5220,16 +5299,16 @@
         <v>15536.865868655899</v>
       </c>
       <c r="AZ61" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA61" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XIOTELC</v>
       </c>
       <c r="BB61">
-        <f t="shared" si="9"/>
-        <v>17090.552455521491</v>
+        <f t="shared" si="10"/>
+        <v>15536.865868655899</v>
       </c>
       <c r="BJ61">
         <v>1</v>
@@ -5245,27 +5324,27 @@
       </c>
       <c r="G62" s="6">
         <f>G61</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="H62" s="6">
-        <f t="shared" si="25"/>
-        <v>0.76100000000000001</v>
+        <f t="shared" si="28"/>
+        <v>0.76065573770491801</v>
       </c>
       <c r="I62" s="15">
-        <f t="shared" si="25"/>
-        <v>0.76100000000000001</v>
+        <f t="shared" si="28"/>
+        <v>0.76065573770491801</v>
       </c>
       <c r="J62" s="15">
         <f>J61</f>
-        <v>0.78700000000000003</v>
+        <v>0.78098360655737697</v>
       </c>
       <c r="K62" s="15">
-        <f t="shared" si="26"/>
-        <v>0.78700000000000003</v>
+        <f t="shared" si="29"/>
+        <v>0.78098360655737697</v>
       </c>
       <c r="L62" s="15">
-        <f t="shared" si="26"/>
-        <v>0.78700000000000003</v>
+        <f t="shared" si="29"/>
+        <v>0.78098360655737697</v>
       </c>
       <c r="T62" s="9" t="s">
         <v>97</v>
@@ -5283,16 +5362,16 @@
         <v>15536.865868655899</v>
       </c>
       <c r="AZ62" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA62" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XIPPELC</v>
       </c>
       <c r="BB62">
-        <f t="shared" si="9"/>
-        <v>17090.552455521491</v>
+        <f t="shared" si="10"/>
+        <v>15536.865868655899</v>
       </c>
       <c r="BJ62">
         <v>1</v>
@@ -5308,27 +5387,27 @@
       </c>
       <c r="G63" s="6">
         <f>G62</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="H63" s="6">
         <f>H62</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="I63" s="6">
         <f>H63</f>
-        <v>0.76100000000000001</v>
+        <v>0.76065573770491801</v>
       </c>
       <c r="J63" s="6">
-        <f t="shared" ref="J63" si="27">I63</f>
-        <v>0.76100000000000001</v>
+        <f t="shared" ref="J63" si="30">I63</f>
+        <v>0.76065573770491801</v>
       </c>
       <c r="K63" s="6">
-        <f t="shared" si="26"/>
-        <v>0.76100000000000001</v>
+        <f t="shared" si="29"/>
+        <v>0.76065573770491801</v>
       </c>
       <c r="L63" s="6">
-        <f t="shared" si="26"/>
-        <v>0.76100000000000001</v>
+        <f t="shared" si="29"/>
+        <v>0.76065573770491801</v>
       </c>
       <c r="N63" t="s">
         <v>128</v>
@@ -5349,16 +5428,16 @@
         <v>40688.264738559599</v>
       </c>
       <c r="AZ63" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA63" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XRESELC</v>
       </c>
       <c r="BB63">
-        <f t="shared" si="9"/>
-        <v>44757.091212415566</v>
+        <f t="shared" si="10"/>
+        <v>40688.264738559599</v>
       </c>
       <c r="BJ63">
         <v>1</v>
@@ -5381,22 +5460,25 @@
         <v>20344.132435184001</v>
       </c>
       <c r="AZ64" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA64" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XTRAELC</v>
       </c>
       <c r="BB64">
-        <f t="shared" si="9"/>
-        <v>22378.545678702401</v>
+        <f t="shared" si="10"/>
+        <v>20344.132435184001</v>
       </c>
       <c r="BJ64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="20:62" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:62" x14ac:dyDescent="0.25">
+      <c r="C65" s="10" t="s">
+        <v>135</v>
+      </c>
       <c r="T65" s="9" t="s">
         <v>103</v>
       </c>
@@ -5413,26 +5495,194 @@
         <v>10172.066217592001</v>
       </c>
       <c r="AZ65" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>NCAP_COST</v>
       </c>
       <c r="BA65" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>XUPSELC</v>
       </c>
       <c r="BB65">
-        <f t="shared" si="9"/>
-        <v>11189.272839351201</v>
+        <f t="shared" si="10"/>
+        <v>10172.066217592001</v>
       </c>
       <c r="BJ65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="20:62" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:62" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>112</v>
+      </c>
+      <c r="G66" s="6">
+        <v>0</v>
+      </c>
+      <c r="H66" s="6">
+        <v>0</v>
+      </c>
+      <c r="I66" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="J66" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="K66" s="6">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L66" s="6">
+        <v>0.1</v>
+      </c>
       <c r="V66" s="9"/>
       <c r="W66" s="9"/>
     </row>
+    <row r="67" spans="3:62" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>113</v>
+      </c>
+      <c r="G67" s="6">
+        <v>0</v>
+      </c>
+      <c r="H67" s="6">
+        <v>0</v>
+      </c>
+      <c r="I67" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="J67" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="K67" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="L67" s="6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="68" spans="3:62" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>114</v>
+      </c>
+      <c r="G68" s="6">
+        <v>0</v>
+      </c>
+      <c r="H68" s="6">
+        <v>0</v>
+      </c>
+      <c r="I68" s="28">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J68" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="K68" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="L68" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="69" spans="3:62" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>127</v>
+      </c>
+      <c r="G69" s="6">
+        <v>0</v>
+      </c>
+      <c r="H69" s="6">
+        <v>0</v>
+      </c>
+      <c r="I69" s="6">
+        <v>0</v>
+      </c>
+      <c r="J69" s="6">
+        <v>0</v>
+      </c>
+      <c r="K69" s="6">
+        <v>0</v>
+      </c>
+      <c r="L69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="3:62" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>130</v>
+      </c>
+      <c r="H79" t="s">
+        <v>131</v>
+      </c>
+      <c r="I79" t="s">
+        <v>9</v>
+      </c>
+      <c r="J79" t="s">
+        <v>132</v>
+      </c>
+      <c r="K79" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="3:62" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>129</v>
+      </c>
+      <c r="G80">
+        <v>100</v>
+      </c>
+      <c r="H80">
+        <v>1524</v>
+      </c>
+      <c r="I80">
+        <f>H80+G80</f>
+        <v>1624</v>
+      </c>
+      <c r="J80">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G81" s="4">
+        <f>G80/I80</f>
+        <v>6.1576354679802957E-2</v>
+      </c>
+      <c r="J81" s="29">
+        <f>J80/I80</f>
+        <v>9.852216748768473E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>134</v>
+      </c>
+      <c r="G82">
+        <v>36.5</v>
+      </c>
+      <c r="H82">
+        <v>116</v>
+      </c>
+      <c r="I82">
+        <f>H82+G82</f>
+        <v>152.5</v>
+      </c>
+      <c r="J82">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="83" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G83" s="29">
+        <f>G82/I82</f>
+        <v>0.23934426229508196</v>
+      </c>
+      <c r="J83" s="29">
+        <f>J82/I82</f>
+        <v>2.0327868852459016E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{28F83205-2B6D-4B86-9C9B-CC3DB94DE282}">
+      <formula1>$F$41:$F$44</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>